<commit_message>
php börjar se fint ut :)
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E22A6E9-7B17-42F9-9C37-9024E475ECD3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0953F27-8865-4506-A06B-840DFC29EECF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="1215" windowWidth="16185" windowHeight="12015" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="1500" yWindow="1560" windowWidth="19035" windowHeight="12015" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +692,7 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="1"/>
       <c r="E10" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Nya länkar och backlog
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0953F27-8865-4506-A06B-840DFC29EECF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF1D350-81D2-4EA7-829F-CC99219F0798}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1560" windowWidth="19035" windowHeight="12015" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="1500" yWindow="1560" windowWidth="22170" windowHeight="12015" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>Uppgift</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t>Sprint</t>
+  </si>
+  <si>
+    <t>Gemensam meny för hemsidan</t>
+  </si>
+  <si>
+    <t>Produktlänkar från databasen</t>
+  </si>
+  <si>
+    <t>Hämta produkter från databasen och genera klickbara länkar till produkterna.</t>
+  </si>
+  <si>
+    <t>Produktkategorier</t>
+  </si>
+  <si>
+    <t>Istället för bara strängar i Products så har vi foreign key till en tabell.</t>
   </si>
 </sst>
 </file>
@@ -541,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B0A93-A15E-478B-B68F-0A6D7C63864A}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,8 +567,9 @@
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="77.42578125" customWidth="1"/>
     <col min="9" max="9" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -571,10 +587,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="I1" t="s">
         <v>19</v>
@@ -693,7 +709,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>30</v>
       </c>
     </row>
@@ -708,7 +724,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -726,51 +742,93 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4"/>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nu har vi stöd för kundkorg och recensioner :)
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{893E5E0C-D203-426B-A227-AC3DDFC8A052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4319CA11-1A17-4878-BAB2-7F7DDB55CDB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="-19320" yWindow="765" windowWidth="19440" windowHeight="15000" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>Uppgift</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Lägg till användarfunktionalitet</t>
-  </si>
-  <si>
-    <t>kolla /index.php</t>
   </si>
   <si>
     <t>Sprint</t>
@@ -594,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B0A93-A15E-478B-B68F-0A6D7C63864A}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +608,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -626,7 +623,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>27</v>
@@ -650,7 +647,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -671,7 +668,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
         <v>20</v>
@@ -692,7 +689,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -700,17 +697,17 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -718,17 +715,17 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -736,7 +733,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -746,7 +743,7 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -754,13 +751,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" t="s">
@@ -772,13 +769,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" t="s">
@@ -800,10 +797,7 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -819,7 +813,10 @@
       <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -834,14 +831,17 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -851,7 +851,7 @@
       </c>
       <c r="E13" s="3"/>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -874,7 +874,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -884,7 +884,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>